<commit_message>
BRVM Realtime & Sectors
</commit_message>
<xml_diff>
--- a/BRVM Excel R files/BRVM_Sectors.xlsx
+++ b/BRVM Excel R files/BRVM_Sectors.xlsx
@@ -413,13 +413,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>106.84</v>
+        <v>107.33</v>
       </c>
       <c r="C2" t="n">
-        <v>106.59</v>
+        <v>107.19</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.23</v>
+        <v>-0.13</v>
       </c>
       <c r="E2" t="n">
         <v>-0.36</v>
@@ -430,13 +430,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>162.38</v>
+        <v>174.28</v>
       </c>
       <c r="C3" t="n">
-        <v>163.42</v>
+        <v>173.58</v>
       </c>
       <c r="D3" t="n">
-        <v>0.64</v>
+        <v>-0.4</v>
       </c>
       <c r="E3" t="n">
         <v>2.09</v>
@@ -447,13 +447,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>931.58</v>
+        <v>993.28</v>
       </c>
       <c r="C4" t="n">
-        <v>993.28</v>
+        <v>943.92</v>
       </c>
       <c r="D4" t="n">
-        <v>6.62</v>
+        <v>-4.97</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -464,13 +464,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>212.07</v>
+        <v>213.8</v>
       </c>
       <c r="C5" t="n">
-        <v>211.92</v>
+        <v>213.43</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.07</v>
+        <v>-0.17</v>
       </c>
       <c r="E5" t="n">
         <v>-0.36</v>
@@ -481,13 +481,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>302.76</v>
+        <v>313.06</v>
       </c>
       <c r="C6" t="n">
-        <v>298.72</v>
+        <v>313.91</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.33</v>
+        <v>0.27</v>
       </c>
       <c r="E6" t="n">
         <v>1.12</v>
@@ -498,13 +498,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>85.98</v>
+        <v>86.82</v>
       </c>
       <c r="C7" t="n">
-        <v>86.52</v>
+        <v>86.37</v>
       </c>
       <c r="D7" t="n">
-        <v>0.63</v>
+        <v>-0.52</v>
       </c>
       <c r="E7" t="n">
         <v>0.45</v>
@@ -515,13 +515,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>100.79</v>
+        <v>102.91</v>
       </c>
       <c r="C8" t="n">
-        <v>100.95</v>
+        <v>101.83</v>
       </c>
       <c r="D8" t="n">
-        <v>0.16</v>
+        <v>-1.05</v>
       </c>
       <c r="E8" t="n">
         <v>-0.65</v>
@@ -532,13 +532,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>99.13</v>
+        <v>99.72</v>
       </c>
       <c r="C9" t="n">
-        <v>98.83</v>
+        <v>99.55</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.3</v>
+        <v>-0.17</v>
       </c>
       <c r="E9" t="n">
         <v>1.05</v>
@@ -549,13 +549,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>102.79</v>
+        <v>104.02</v>
       </c>
       <c r="C10" t="n">
-        <v>102.92</v>
+        <v>103.77</v>
       </c>
       <c r="D10" t="n">
-        <v>0.13</v>
+        <v>-0.24</v>
       </c>
       <c r="E10" t="n">
         <v>-1.06</v>
@@ -566,13 +566,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>526.47</v>
+        <v>524.94</v>
       </c>
       <c r="C11" t="n">
-        <v>523.25</v>
+        <v>526.04</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.61</v>
+        <v>0.21</v>
       </c>
       <c r="E11" t="n">
         <v>-1.18</v>
@@ -583,13 +583,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>366.76</v>
+        <v>373.92</v>
       </c>
       <c r="C12" t="n">
-        <v>372.73</v>
+        <v>377.5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.63</v>
+        <v>0.96</v>
       </c>
       <c r="E12" t="n">
         <v>-3.48</v>

</xml_diff>